<commit_message>
Added Programmer to Budget
</commit_message>
<xml_diff>
--- a/Documentation/Budget 9-22-15.xlsx
+++ b/Documentation/Budget 9-22-15.xlsx
@@ -33,10 +33,10 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Includes FRDM-K22 dev kit</t>
+    <t>Current Measurement</t>
   </si>
   <si>
-    <t>Current Measurement</t>
+    <t>Includes FRDM-K22 dev kit and Segger J-Link EDU</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -541,16 +541,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <f>10+5+30</f>
-        <v>45</v>
+        <f>10+5+30+70</f>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>16</v>

</xml_diff>

<commit_message>
Updated Budget: Power Subsection
</commit_message>
<xml_diff>
--- a/Documentation/Budget 9-22-15.xlsx
+++ b/Documentation/Budget 9-22-15.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>MCU</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Current Measurement</t>
+  </si>
+  <si>
+    <t>Power</t>
   </si>
 </sst>
 </file>
@@ -104,6 +107,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -515,17 +523,17 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.875" customWidth="1"/>
     <col min="3" max="3" width="63.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="90" customHeight="1"/>
-    <row r="3" spans="1:3">
+    <row r="1" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -536,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -548,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -556,127 +564,132 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SD card cost added
</commit_message>
<xml_diff>
--- a/Documentation/Budget 9-22-15.xlsx
+++ b/Documentation/Budget 9-22-15.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>MCU</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>LCD</t>
+  </si>
+  <si>
+    <t>SD Card</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -584,7 +587,12 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>

</xml_diff>

<commit_message>
Design Specifications and Budget updated
Modified Design Specifications to be submitted September 23
</commit_message>
<xml_diff>
--- a/Documentation/Budget 9-22-15.xlsx
+++ b/Documentation/Budget 9-22-15.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>MCU</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>SD Card</t>
+  </si>
+  <si>
+    <t>so far</t>
   </si>
 </sst>
 </file>
@@ -55,7 +58,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,6 +78,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,9 +113,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -180,7 +192,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>EE4951W Initial</a:t>
+            <a:t>EE4951W - Power Monitoring Device - Initial</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -529,7 +541,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -595,7 +607,12 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
+      <c r="B9" s="2">
+        <v>131</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
@@ -710,8 +727,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Design specifications, individual roles and description of demonstration added
</commit_message>
<xml_diff>
--- a/Documentation/Budget 9-22-15.xlsx
+++ b/Documentation/Budget 9-22-15.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>MCU</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>SD Card</t>
-  </si>
-  <si>
-    <t>so far</t>
   </si>
 </sst>
 </file>
@@ -541,7 +538,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -610,9 +607,6 @@
       <c r="B9" s="2">
         <v>131</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>

</xml_diff>